<commit_message>
reconciled part the waterveil and radiant flames in trade binder for standard
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1516" uniqueCount="1506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="1508">
   <si>
     <t>Weldfast Wingsmith</t>
   </si>
@@ -4545,6 +4545,12 @@
   </si>
   <si>
     <t>Plummet</t>
+  </si>
+  <si>
+    <t>Radiant Flames</t>
+  </si>
+  <si>
+    <t>Part the Waterveil</t>
   </si>
 </sst>
 </file>
@@ -4914,11 +4920,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F1511"/>
+  <dimension ref="A1:F1513"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1501" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1512" sqref="F1512"/>
+      <pane ySplit="1" topLeftCell="A1498" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1514" sqref="C1514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17029,6 +17035,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="1512" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1512" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C1512">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1513" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C1513">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1507">
     <filterColumn colId="1">

</xml_diff>

<commit_message>
checked out sol ring and ashnod's altar
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="1520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="1521">
   <si>
     <t>Weldfast Wingsmith</t>
   </si>
@@ -4587,6 +4587,9 @@
   </si>
   <si>
     <t>Paradox Engine</t>
+  </si>
+  <si>
+    <t>Liliana, Defiant Necromancer</t>
   </si>
 </sst>
 </file>
@@ -4959,11 +4962,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1523"/>
+  <dimension ref="A1:H1524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1492" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1524" sqref="C1524"/>
+      <pane ySplit="1" topLeftCell="A1522" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1525" sqref="D1525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17191,6 +17194,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1524" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1524" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D1524">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1518"/>
   <sortState ref="A2:A2143">

</xml_diff>